<commit_message>
Food Listing Page Automation
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeongmeng/foodgrab/src/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yeongmeng/foodgrab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD8010F-F0EB-4043-B1CD-FDC18BC84057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86A171B-292E-1F4F-B307-CF9695C0A083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="2220" windowWidth="27640" windowHeight="16940" xr2:uid="{73DDAD36-3914-C94B-B04B-13C1BD7EA228}"/>
+    <workbookView xWindow="12700" yWindow="8200" windowWidth="27640" windowHeight="16940" xr2:uid="{73DDAD36-3914-C94B-B04B-13C1BD7EA228}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
-  <si>
-    <t>user_id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>username</t>
   </si>
@@ -116,12 +113,6 @@
     <t>abcdefg</t>
   </si>
   <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>business</t>
-  </si>
-  <si>
     <t>Blog4me@gmail.com</t>
   </si>
   <si>
@@ -180,6 +171,9 @@
   </si>
   <si>
     <t>Cherma@gmail.com</t>
+  </si>
+  <si>
+    <t>rating</t>
   </si>
 </sst>
 </file>
@@ -534,13 +528,13 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -557,347 +551,347 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E13">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="E17">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="E20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
+      <c r="E21">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>